<commit_message>
added new results to excel
</commit_message>
<xml_diff>
--- a/Results/TM-TestResults/ComputeTime TM Algorithms 40000 columns/TopologyComputeSpeed SP with TM.xlsx
+++ b/Results/TM-TestResults/ComputeTime TM Algorithms 40000 columns/TopologyComputeSpeed SP with TM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\neocortexapi\neocortexapi\Results\TM-TestResults\ComputeTime TM Algorithms 40000 columns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14C27F8-8ED0-464C-B62F-6715AC3C5FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2168FC02-E758-4FE1-944F-1F442515C870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-10128" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{697608A7-46EB-44DA-9169-295BAC6E2D80}"/>
   </bookViews>
@@ -39,26 +39,27 @@
     <definedName name="_xlchart.v1.24" hidden="1">'Topology Perfoemance 2'!$E$1:$E$1185</definedName>
     <definedName name="_xlchart.v1.25" hidden="1">'Topology Perfoemance 2'!$F$1:$F$1185</definedName>
     <definedName name="_xlchart.v1.26" hidden="1">'Topology Perfoemance 2'!$G$1:$G$1185</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'Topology Perfoemance 2'!$A$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'Topology Perfoemance 2'!$A$2:$A$1185</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'Topology Perfoemance 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'Topology Perfoemance 2'!$L$2:$Q$2</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'Topology Perfoemance 2'!$A$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'Topology Perfoemance 2'!$A$2:$A$1185</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'Topology Performance'!$D$2:$D$172</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'Topology Perfoemance 2'!$B$2:$B$1185</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'Topology Perfoemance 2'!$B:$B</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'Topology Perfoemance 2'!$C$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'Topology Perfoemance 2'!$C$2:$C$1185</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'Topology Perfoemance 2'!$D$1</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'Topology Perfoemance 2'!$D$2:$D$1185</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'Topology Perfoemance 2'!$E$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'Topology Perfoemance 2'!$E$2:$E$1185</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'Topology Perfoemance 2'!$F$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'Topology Perfoemance 2'!$F:$F</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'Topology Perfoemance 2'!$B$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'Topology Perfoemance 2'!$B$2:$B$1185</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'Topology Perfoemance 2'!$B:$B</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'Topology Perfoemance 2'!$C$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'Topology Perfoemance 2'!$C$2:$C$1185</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'Topology Perfoemance 2'!$D$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'Topology Perfoemance 2'!$D$2:$D$1185</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'Topology Perfoemance 2'!$E$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'Topology Perfoemance 2'!$E$2:$E$1185</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'Topology Perfoemance 2'!$F$1</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Topology Performance'!$E$2:$E$172</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'Topology Perfoemance 2'!$G$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'Topology Perfoemance 2'!$G:$G</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">('Topology Perfoemance 2'!$A:$A,'Topology Perfoemance 2'!$A$1)</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'Algorithm Performance'!$A$2:$A$2516</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'Algorithm Performance'!$B$2:$B$2516</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'Topology Perfoemance 2'!$F:$F</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'Topology Perfoemance 2'!$G$1</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'Topology Perfoemance 2'!$G:$G</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">('Topology Perfoemance 2'!$A:$A,'Topology Perfoemance 2'!$A$1)</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'Algorithm Performance'!$A$2:$A$2516</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">'Algorithm Performance'!$B$2:$B$2516</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Topology Performance'!$A$2:$A$115</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'Topology Performance'!$B$2:$B$115</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'Topology Performance'!$C$2:$C$115</definedName>
@@ -582,13 +583,159 @@
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.27</cx:f>
+      </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.43</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.22</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.23</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.24</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="5">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.25</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="6">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.26</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="1" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>tm.compute()</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t> time as a function of a number of mini-columns</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{02813925-9D94-484E-B68C-3ACEF58A45BF}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{D3804A09-826A-4184-BE1C-20B5A7CD7D24}">
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2E87DB2D-B7E2-4365-87AD-B1C6C11EB7DC}">
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{254B97FD-DF14-4C01-84D8-247E8AEC6080}">
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{D7F628AC-BB46-4FD1-B446-B8B43A534265}">
+          <cx:dataId val="4"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{674C6F20-0E8F-445C-A280-0B96C290721E}">
+          <cx:dataId val="5"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{7C36061D-A922-4FF5-91FE-A2FF430CB386}">
+          <cx:dataId val="6"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="inclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
         <cx:f>_xlchart.v1.44</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.45</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -813,6 +960,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3427,6 +3614,521 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3717,6 +4419,84 @@
             <a:xfrm>
               <a:off x="10233660" y="2644140"/>
               <a:ext cx="5280660" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-DE" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>441007</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>31432</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>541972</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>31432</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Chart 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACB42FF6-93C3-40F6-BC6F-415ABD3AB8EA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10286047" y="6066472"/>
+              <a:ext cx="5282565" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -26641,10 +27421,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5324C0A-4B86-4581-AFE7-D2D4261A0B0A}">
-  <dimension ref="A1:G1185"/>
+  <dimension ref="A1:Q1185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26656,7 +27436,7 @@
     <col min="7" max="7" width="9.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -26676,7 +27456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>95</v>
       </c>
@@ -26698,8 +27478,26 @@
       <c r="G2" s="2">
         <v>4656</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="L2">
+        <v>2048</v>
+      </c>
+      <c r="M2">
+        <v>4096</v>
+      </c>
+      <c r="N2">
+        <v>8612</v>
+      </c>
+      <c r="O2">
+        <v>16384</v>
+      </c>
+      <c r="P2">
+        <v>40000</v>
+      </c>
+      <c r="Q2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>67</v>
       </c>
@@ -26722,7 +27520,7 @@
         <v>6471</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>111</v>
       </c>
@@ -26745,7 +27543,7 @@
         <v>12777</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>93</v>
       </c>
@@ -26768,7 +27566,7 @@
         <v>14399</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>66</v>
       </c>
@@ -26791,7 +27589,7 @@
         <v>10081</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>103</v>
       </c>
@@ -26814,7 +27612,7 @@
         <v>14076</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>111</v>
       </c>
@@ -26837,7 +27635,7 @@
         <v>14724</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>104</v>
       </c>
@@ -26860,7 +27658,7 @@
         <v>15069</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>99</v>
       </c>
@@ -26883,7 +27681,7 @@
         <v>9838</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>115</v>
       </c>
@@ -26906,7 +27704,7 @@
         <v>15809</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>143</v>
       </c>
@@ -26929,7 +27727,7 @@
         <v>21332</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>123</v>
       </c>
@@ -26952,7 +27750,7 @@
         <v>17764</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>94</v>
       </c>
@@ -26975,7 +27773,7 @@
         <v>11422</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>94</v>
       </c>
@@ -26998,7 +27796,7 @@
         <v>20269</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>86</v>
       </c>

</xml_diff>